<commit_message>
Improve preservation of unit cases for custom units
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_seasonal_test.xlsx
+++ b/tests/frameworks/framework_seasonal_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BB8F5E-7CA8-432F-B371-A984A7BDB164}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48235B98-EDBA-44A6-AB55-535A93C6D9B1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -687,9 +687,6 @@
     <t>number/mm</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>dead</t>
   </si>
   <si>
@@ -721,6 +718,9 @@
   </si>
   <si>
     <t>(seasonal_min+seasonal_max)/2+(seasonal_max-seasonal_min)/2*cos(t*2*pi+pi)</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
 </sst>
 </file>
@@ -1408,10 +1408,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>31</v>
@@ -1509,7 +1509,7 @@
         <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="3" t="str">
         <f>IF(Compartments!$A12&lt;&gt;"",Compartments!$A12,"")</f>
@@ -3065,12 +3065,12 @@
         <v>34</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:389" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:389" x14ac:dyDescent="0.25">
@@ -5547,7 +5547,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5629,10 +5629,10 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5647,10 +5647,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5670,7 +5670,7 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -5681,21 +5681,21 @@
         <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="6">
         <v>0.4</v>

</xml_diff>